<commit_message>
add reading from excel
</commit_message>
<xml_diff>
--- a/gamsWorkSpace/aerzte.xlsx
+++ b/gamsWorkSpace/aerzte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\itStud9Lp2024\gamsWorkSpace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104044CB-D2B5-4DB8-A9E4-3E491D24EAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D12103-9A7F-4EB1-87FE-C9AC6BD358AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC869186-945C-4085-8A53-86DCFD75D10A}"/>
+    <workbookView xWindow="3480" yWindow="5100" windowWidth="21600" windowHeight="11295" xr2:uid="{BC869186-945C-4085-8A53-86DCFD75D10A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>231</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>223</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>232</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="C16">
-        <v>23</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>535</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>223</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="C21">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>